<commit_message>
:art: Refactor evaluation code. Fixed a bug: Entropy compute error
An entropy compute error occurred within the binary analysis part. Duplicate computed negative condition part while leaving positive part, yielding a pretty strange error. Fixed after refactoring.
</commit_message>
<xml_diff>
--- a/rotten_tomatoes/movie_list/movie_data.xlsx
+++ b/rotten_tomatoes/movie_list/movie_data.xlsx
@@ -8,15 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangyanzhen/Developer/GitHub/CISC3014-IR-and-WebSearch-Project/rotten_tomatoes/movie_list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{3C537E41-B9F6-0846-B4A4-969D80A5E22C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C530F9E-569B-584E-AF22-F3FE4067D7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24500" yWindow="2720" windowWidth="30240" windowHeight="18880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1113,15 +1112,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1433,14 +1431,14 @@
   <dimension ref="A1:H120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="P36" sqref="P36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="43.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="6" max="6" width="9.1640625" customWidth="1"/>
     <col min="7" max="7" width="26.1640625" customWidth="1"/>
@@ -1468,7 +1466,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="5" t="s">
+      <c r="H1" s="4" t="s">
         <v>331</v>
       </c>
     </row>
@@ -1482,10 +1480,10 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>88</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E2">
         <v>26</v>
       </c>
       <c r="F2">
@@ -1505,10 +1503,10 @@
       <c r="C3" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3">
         <v>70</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>23</v>
       </c>
       <c r="F3">
@@ -1528,10 +1526,10 @@
       <c r="C4" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4">
         <v>87</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>71</v>
       </c>
       <c r="F4">
@@ -1551,10 +1549,10 @@
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5">
         <v>59</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>22</v>
       </c>
       <c r="F5">
@@ -1574,10 +1572,10 @@
       <c r="C6" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6">
         <v>82</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>94</v>
       </c>
       <c r="F6">
@@ -1597,10 +1595,10 @@
       <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7">
         <v>89</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>79</v>
       </c>
       <c r="F7">
@@ -1620,10 +1618,10 @@
       <c r="C8" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8">
         <v>83</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>91</v>
       </c>
       <c r="F8">
@@ -1643,7 +1641,7 @@
       <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9">
         <v>85</v>
       </c>
       <c r="E9">
@@ -1666,10 +1664,10 @@
       <c r="C10" t="s">
         <v>30</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10">
         <v>75</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E10">
         <v>96</v>
       </c>
       <c r="F10">
@@ -1689,10 +1687,10 @@
       <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11">
         <v>57</v>
       </c>
-      <c r="E11" s="2">
+      <c r="E11">
         <v>99</v>
       </c>
       <c r="F11">
@@ -1712,10 +1710,10 @@
       <c r="C12" t="s">
         <v>35</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12">
         <v>95</v>
       </c>
-      <c r="E12" s="2">
+      <c r="E12">
         <v>59</v>
       </c>
       <c r="F12">
@@ -1735,10 +1733,10 @@
       <c r="C13" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13">
         <v>52</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13">
         <v>86</v>
       </c>
       <c r="F13">
@@ -1758,10 +1756,10 @@
       <c r="C14" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14">
         <v>77</v>
       </c>
-      <c r="E14" s="2">
+      <c r="E14">
         <v>88</v>
       </c>
       <c r="F14">
@@ -1781,10 +1779,10 @@
       <c r="C15" t="s">
         <v>43</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15">
         <v>71</v>
       </c>
-      <c r="E15" s="2">
+      <c r="E15">
         <v>44</v>
       </c>
       <c r="F15">
@@ -1804,10 +1802,10 @@
       <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16">
         <v>73</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E16">
         <v>52</v>
       </c>
       <c r="F16">
@@ -1827,10 +1825,10 @@
       <c r="C17" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17">
         <v>68</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17">
         <v>82</v>
       </c>
       <c r="F17">
@@ -1850,10 +1848,10 @@
       <c r="C18" t="s">
         <v>51</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18">
         <v>84</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18">
         <v>37</v>
       </c>
       <c r="F18">
@@ -1873,10 +1871,10 @@
       <c r="C19" t="s">
         <v>54</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19">
         <v>82</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19">
         <v>95</v>
       </c>
       <c r="F19">
@@ -1896,10 +1894,10 @@
       <c r="C20" t="s">
         <v>57</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20">
         <v>56</v>
       </c>
-      <c r="E20" s="2">
+      <c r="E20">
         <v>82</v>
       </c>
       <c r="F20">
@@ -1919,10 +1917,10 @@
       <c r="C21" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21">
         <v>94</v>
       </c>
-      <c r="E21" s="2">
+      <c r="E21">
         <v>96</v>
       </c>
       <c r="F21">
@@ -1942,10 +1940,10 @@
       <c r="C22" t="s">
         <v>63</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22">
         <v>77</v>
       </c>
-      <c r="E22" s="2">
+      <c r="E22">
         <v>75</v>
       </c>
       <c r="F22">
@@ -1965,10 +1963,10 @@
       <c r="C23" t="s">
         <v>66</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23">
         <v>67</v>
       </c>
-      <c r="E23" s="2">
+      <c r="E23">
         <v>97</v>
       </c>
       <c r="F23">
@@ -1988,10 +1986,10 @@
       <c r="C24" t="s">
         <v>68</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24">
         <v>83</v>
       </c>
-      <c r="E24" s="2">
+      <c r="E24">
         <v>88</v>
       </c>
       <c r="F24">
@@ -2011,10 +2009,10 @@
       <c r="C25" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25">
         <v>92</v>
       </c>
-      <c r="E25" s="2">
+      <c r="E25">
         <v>98</v>
       </c>
       <c r="F25">
@@ -2034,10 +2032,10 @@
       <c r="C26" t="s">
         <v>73</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26">
         <v>94</v>
       </c>
-      <c r="E26" s="2">
+      <c r="E26">
         <v>75</v>
       </c>
       <c r="F26">
@@ -2057,10 +2055,10 @@
       <c r="C27" t="s">
         <v>76</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27">
         <v>74</v>
       </c>
-      <c r="E27" s="2">
+      <c r="E27">
         <v>82</v>
       </c>
       <c r="F27">
@@ -2080,10 +2078,10 @@
       <c r="C28" t="s">
         <v>79</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28">
         <v>41</v>
       </c>
-      <c r="E28" s="2">
+      <c r="E28">
         <v>25</v>
       </c>
       <c r="F28">
@@ -2103,10 +2101,10 @@
       <c r="C29" t="s">
         <v>82</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29">
         <v>40</v>
       </c>
-      <c r="E29" s="2">
+      <c r="E29">
         <v>15</v>
       </c>
       <c r="F29">
@@ -2126,10 +2124,10 @@
       <c r="C30" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30">
         <v>59</v>
       </c>
-      <c r="E30" s="2">
+      <c r="E30">
         <v>95</v>
       </c>
       <c r="F30">
@@ -2149,10 +2147,10 @@
       <c r="C31" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31">
         <v>73</v>
       </c>
-      <c r="E31" s="2">
+      <c r="E31">
         <v>92</v>
       </c>
       <c r="F31">
@@ -2172,10 +2170,10 @@
       <c r="C32" t="s">
         <v>94</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32">
         <v>78</v>
       </c>
-      <c r="E32" s="2">
+      <c r="E32">
         <v>93</v>
       </c>
       <c r="F32">
@@ -2195,10 +2193,10 @@
       <c r="C33" t="s">
         <v>97</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33">
         <v>75</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E33">
         <v>94</v>
       </c>
       <c r="F33">
@@ -2218,10 +2216,10 @@
       <c r="C34" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34">
         <v>99</v>
       </c>
-      <c r="E34" s="2">
+      <c r="E34">
         <v>58</v>
       </c>
       <c r="F34">
@@ -2241,10 +2239,10 @@
       <c r="C35" t="s">
         <v>102</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35">
         <v>66</v>
       </c>
-      <c r="E35" s="2">
+      <c r="E35">
         <v>60</v>
       </c>
       <c r="F35">
@@ -2264,10 +2262,10 @@
       <c r="C36" t="s">
         <v>105</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36">
         <v>86</v>
       </c>
-      <c r="E36" s="2">
+      <c r="E36">
         <v>98</v>
       </c>
       <c r="F36">
@@ -2287,10 +2285,10 @@
       <c r="C37" t="s">
         <v>108</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37">
         <v>92</v>
       </c>
-      <c r="E37" s="2">
+      <c r="E37">
         <v>95</v>
       </c>
       <c r="F37">
@@ -2310,10 +2308,10 @@
       <c r="C38" t="s">
         <v>111</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38">
         <v>92</v>
       </c>
-      <c r="E38" s="2">
+      <c r="E38">
         <v>78</v>
       </c>
       <c r="F38">
@@ -2333,10 +2331,10 @@
       <c r="C39" t="s">
         <v>114</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39">
         <v>76</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E39">
         <v>84</v>
       </c>
       <c r="F39">
@@ -2356,10 +2354,10 @@
       <c r="C40" t="s">
         <v>117</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40">
         <v>70</v>
       </c>
-      <c r="E40" s="2">
+      <c r="E40">
         <v>90</v>
       </c>
       <c r="F40">
@@ -2379,10 +2377,10 @@
       <c r="C41" t="s">
         <v>120</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41">
         <v>68</v>
       </c>
-      <c r="E41" s="2">
+      <c r="E41">
         <v>61</v>
       </c>
       <c r="F41">
@@ -2402,10 +2400,10 @@
       <c r="C42" t="s">
         <v>123</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42">
         <v>94</v>
       </c>
-      <c r="E42" s="2">
+      <c r="E42">
         <v>96</v>
       </c>
       <c r="F42">
@@ -2425,10 +2423,10 @@
       <c r="C43" t="s">
         <v>125</v>
       </c>
-      <c r="D43" s="2">
+      <c r="D43">
         <v>88</v>
       </c>
-      <c r="E43" s="2">
+      <c r="E43">
         <v>86</v>
       </c>
       <c r="F43">
@@ -2448,10 +2446,10 @@
       <c r="C44" t="s">
         <v>128</v>
       </c>
-      <c r="D44" s="2">
+      <c r="D44">
         <v>61</v>
       </c>
-      <c r="E44" s="2">
+      <c r="E44">
         <v>21</v>
       </c>
       <c r="F44">
@@ -2471,10 +2469,10 @@
       <c r="C45" t="s">
         <v>131</v>
       </c>
-      <c r="D45" s="2">
+      <c r="D45">
         <v>89</v>
       </c>
-      <c r="E45" s="2">
+      <c r="E45">
         <v>89</v>
       </c>
       <c r="F45">
@@ -2494,10 +2492,10 @@
       <c r="C46" t="s">
         <v>134</v>
       </c>
-      <c r="D46" s="2">
+      <c r="D46">
         <v>52</v>
       </c>
-      <c r="E46" s="2">
+      <c r="E46">
         <v>87</v>
       </c>
       <c r="F46">
@@ -2517,10 +2515,10 @@
       <c r="C47" t="s">
         <v>136</v>
       </c>
-      <c r="D47" s="2">
+      <c r="D47">
         <v>98</v>
       </c>
-      <c r="E47" s="2">
+      <c r="E47">
         <v>65</v>
       </c>
       <c r="F47">
@@ -2540,10 +2538,10 @@
       <c r="C48" t="s">
         <v>138</v>
       </c>
-      <c r="D48" s="2">
+      <c r="D48">
         <v>53</v>
       </c>
-      <c r="E48" s="2">
+      <c r="E48">
         <v>70</v>
       </c>
       <c r="F48">
@@ -2563,10 +2561,10 @@
       <c r="C49" t="s">
         <v>141</v>
       </c>
-      <c r="D49" s="2">
+      <c r="D49">
         <v>14</v>
       </c>
-      <c r="E49" s="2">
+      <c r="E49">
         <v>87</v>
       </c>
       <c r="F49">
@@ -2586,10 +2584,10 @@
       <c r="C50" t="s">
         <v>143</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50">
         <v>98</v>
       </c>
-      <c r="E50" s="2">
+      <c r="E50">
         <v>83</v>
       </c>
       <c r="F50">
@@ -2609,10 +2607,10 @@
       <c r="C51" t="s">
         <v>146</v>
       </c>
-      <c r="D51" s="2">
+      <c r="D51">
         <v>71</v>
       </c>
-      <c r="E51" s="2">
+      <c r="E51">
         <v>93</v>
       </c>
       <c r="F51">
@@ -2632,10 +2630,10 @@
       <c r="C52" t="s">
         <v>149</v>
       </c>
-      <c r="D52" s="2">
+      <c r="D52">
         <v>81</v>
       </c>
-      <c r="E52" s="2">
+      <c r="E52">
         <v>49</v>
       </c>
       <c r="F52">
@@ -2655,10 +2653,10 @@
       <c r="C53" t="s">
         <v>151</v>
       </c>
-      <c r="D53" s="2">
+      <c r="D53">
         <v>79</v>
       </c>
-      <c r="E53" s="2">
+      <c r="E53">
         <v>58</v>
       </c>
       <c r="F53">
@@ -2678,10 +2676,10 @@
       <c r="C54" t="s">
         <v>154</v>
       </c>
-      <c r="D54" s="2">
+      <c r="D54">
         <v>74</v>
       </c>
-      <c r="E54" s="2">
+      <c r="E54">
         <v>87</v>
       </c>
       <c r="F54">
@@ -2701,10 +2699,10 @@
       <c r="C55" t="s">
         <v>159</v>
       </c>
-      <c r="D55" s="2">
+      <c r="D55">
         <v>82</v>
       </c>
-      <c r="E55" s="2">
+      <c r="E55">
         <v>93</v>
       </c>
       <c r="F55">
@@ -2724,10 +2722,10 @@
       <c r="C56" t="s">
         <v>162</v>
       </c>
-      <c r="D56" s="2">
+      <c r="D56">
         <v>89</v>
       </c>
-      <c r="E56" s="2">
+      <c r="E56">
         <v>32</v>
       </c>
       <c r="F56">
@@ -2747,10 +2745,10 @@
       <c r="C57" t="s">
         <v>165</v>
       </c>
-      <c r="D57" s="2">
+      <c r="D57">
         <v>35</v>
       </c>
-      <c r="E57" s="2">
+      <c r="E57">
         <v>24</v>
       </c>
       <c r="F57">
@@ -2770,10 +2768,10 @@
       <c r="C58" t="s">
         <v>167</v>
       </c>
-      <c r="D58" s="2">
+      <c r="D58">
         <v>50</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E58">
         <v>21</v>
       </c>
       <c r="F58">
@@ -2793,10 +2791,10 @@
       <c r="C59" t="s">
         <v>170</v>
       </c>
-      <c r="D59" s="2">
+      <c r="D59">
         <v>50</v>
       </c>
-      <c r="E59" s="2">
+      <c r="E59">
         <v>38</v>
       </c>
       <c r="F59">
@@ -2816,10 +2814,10 @@
       <c r="C60" t="s">
         <v>172</v>
       </c>
-      <c r="D60" s="2">
+      <c r="D60">
         <v>72</v>
       </c>
-      <c r="E60" s="2">
+      <c r="E60">
         <v>40</v>
       </c>
       <c r="F60">
@@ -2839,10 +2837,10 @@
       <c r="C61" t="s">
         <v>174</v>
       </c>
-      <c r="D61" s="2">
+      <c r="D61">
         <v>71</v>
       </c>
-      <c r="E61" s="2">
+      <c r="E61">
         <v>14</v>
       </c>
       <c r="F61">
@@ -2862,10 +2860,10 @@
       <c r="C62" t="s">
         <v>177</v>
       </c>
-      <c r="D62" s="2">
+      <c r="D62">
         <v>73</v>
       </c>
-      <c r="E62" s="2">
+      <c r="E62">
         <v>100</v>
       </c>
       <c r="F62">
@@ -2885,10 +2883,10 @@
       <c r="C63" t="s">
         <v>180</v>
       </c>
-      <c r="D63" s="2">
+      <c r="D63">
         <v>84</v>
       </c>
-      <c r="E63" s="2">
+      <c r="E63">
         <v>50</v>
       </c>
       <c r="F63">
@@ -2908,10 +2906,10 @@
       <c r="C64" t="s">
         <v>182</v>
       </c>
-      <c r="D64" s="2">
+      <c r="D64">
         <v>93</v>
       </c>
-      <c r="E64" s="2">
+      <c r="E64">
         <v>74</v>
       </c>
       <c r="F64">
@@ -2931,10 +2929,10 @@
       <c r="C65" t="s">
         <v>185</v>
       </c>
-      <c r="D65" s="2">
+      <c r="D65">
         <v>94</v>
       </c>
-      <c r="E65" s="2">
+      <c r="E65">
         <v>98</v>
       </c>
       <c r="F65">
@@ -2954,10 +2952,10 @@
       <c r="C66" t="s">
         <v>188</v>
       </c>
-      <c r="D66" s="2">
+      <c r="D66">
         <v>75</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E66">
         <v>37</v>
       </c>
       <c r="F66">
@@ -2977,10 +2975,10 @@
       <c r="C67" t="s">
         <v>190</v>
       </c>
-      <c r="D67" s="2">
+      <c r="D67">
         <v>75</v>
       </c>
-      <c r="E67" s="2">
+      <c r="E67">
         <v>49</v>
       </c>
       <c r="F67">
@@ -3000,10 +2998,10 @@
       <c r="C68" t="s">
         <v>192</v>
       </c>
-      <c r="D68" s="2">
+      <c r="D68">
         <v>54</v>
       </c>
-      <c r="E68" s="2">
+      <c r="E68">
         <v>13</v>
       </c>
       <c r="F68">
@@ -3023,10 +3021,10 @@
       <c r="C69" t="s">
         <v>195</v>
       </c>
-      <c r="D69" s="2">
+      <c r="D69">
         <v>60</v>
       </c>
-      <c r="E69" s="2">
+      <c r="E69">
         <v>93</v>
       </c>
       <c r="F69">
@@ -3046,10 +3044,10 @@
       <c r="C70" t="s">
         <v>198</v>
       </c>
-      <c r="D70" s="2">
+      <c r="D70">
         <v>89</v>
       </c>
-      <c r="E70" s="2">
+      <c r="E70">
         <v>96</v>
       </c>
       <c r="F70">
@@ -3069,10 +3067,10 @@
       <c r="C71" t="s">
         <v>201</v>
       </c>
-      <c r="D71" s="2">
+      <c r="D71">
         <v>65</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E71">
         <v>18</v>
       </c>
       <c r="F71">
@@ -3092,10 +3090,10 @@
       <c r="C72" t="s">
         <v>203</v>
       </c>
-      <c r="D72" s="2">
+      <c r="D72">
         <v>69</v>
       </c>
-      <c r="E72" s="2">
+      <c r="E72">
         <v>62</v>
       </c>
       <c r="F72">
@@ -3115,10 +3113,10 @@
       <c r="C73" t="s">
         <v>206</v>
       </c>
-      <c r="D73" s="2">
+      <c r="D73">
         <v>91</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E73">
         <v>76</v>
       </c>
       <c r="F73">
@@ -3138,10 +3136,10 @@
       <c r="C74" t="s">
         <v>209</v>
       </c>
-      <c r="D74" s="2">
+      <c r="D74">
         <v>73</v>
       </c>
-      <c r="E74" s="2">
+      <c r="E74">
         <v>28</v>
       </c>
       <c r="F74">
@@ -3161,10 +3159,10 @@
       <c r="C75" t="s">
         <v>211</v>
       </c>
-      <c r="D75" s="2">
+      <c r="D75">
         <v>88</v>
       </c>
-      <c r="E75" s="2">
+      <c r="E75">
         <v>69</v>
       </c>
       <c r="F75">
@@ -3184,10 +3182,10 @@
       <c r="C76" t="s">
         <v>213</v>
       </c>
-      <c r="D76" s="2">
+      <c r="D76">
         <v>89</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E76">
         <v>98</v>
       </c>
       <c r="F76">
@@ -3207,10 +3205,10 @@
       <c r="C77" t="s">
         <v>216</v>
       </c>
-      <c r="D77" s="2">
+      <c r="D77">
         <v>62</v>
       </c>
-      <c r="E77" s="2">
+      <c r="E77">
         <v>33</v>
       </c>
       <c r="F77">
@@ -3230,10 +3228,10 @@
       <c r="C78" t="s">
         <v>219</v>
       </c>
-      <c r="D78" s="2">
+      <c r="D78">
         <v>77</v>
       </c>
-      <c r="E78" s="2">
+      <c r="E78">
         <v>79</v>
       </c>
       <c r="F78">
@@ -3253,10 +3251,10 @@
       <c r="C79" t="s">
         <v>222</v>
       </c>
-      <c r="D79" s="2">
+      <c r="D79">
         <v>85</v>
       </c>
-      <c r="E79" s="2">
+      <c r="E79">
         <v>87</v>
       </c>
       <c r="F79">
@@ -3276,10 +3274,10 @@
       <c r="C80" t="s">
         <v>225</v>
       </c>
-      <c r="D80" s="2">
+      <c r="D80">
         <v>71</v>
       </c>
-      <c r="E80" s="2">
+      <c r="E80">
         <v>99</v>
       </c>
       <c r="F80">
@@ -3299,10 +3297,10 @@
       <c r="C81" t="s">
         <v>228</v>
       </c>
-      <c r="D81" s="2">
+      <c r="D81">
         <v>95</v>
       </c>
-      <c r="E81" s="2">
+      <c r="E81">
         <v>99</v>
       </c>
       <c r="F81">
@@ -3322,10 +3320,10 @@
       <c r="C82" t="s">
         <v>231</v>
       </c>
-      <c r="D82" s="2">
+      <c r="D82">
         <v>93</v>
       </c>
-      <c r="E82" s="2">
+      <c r="E82">
         <v>75</v>
       </c>
       <c r="F82">
@@ -3345,10 +3343,10 @@
       <c r="C83" t="s">
         <v>233</v>
       </c>
-      <c r="D83" s="2">
+      <c r="D83">
         <v>70</v>
       </c>
-      <c r="E83" s="2">
+      <c r="E83">
         <v>71</v>
       </c>
       <c r="F83">
@@ -3368,10 +3366,10 @@
       <c r="C84" t="s">
         <v>236</v>
       </c>
-      <c r="D84" s="2">
+      <c r="D84">
         <v>90</v>
       </c>
-      <c r="E84" s="2">
+      <c r="E84">
         <v>96</v>
       </c>
       <c r="F84">
@@ -3391,10 +3389,10 @@
       <c r="C85" t="s">
         <v>239</v>
       </c>
-      <c r="D85" s="2">
+      <c r="D85">
         <v>72</v>
       </c>
-      <c r="E85" s="2">
+      <c r="E85">
         <v>82</v>
       </c>
       <c r="F85">
@@ -3414,10 +3412,10 @@
       <c r="C86" t="s">
         <v>242</v>
       </c>
-      <c r="D86" s="2">
+      <c r="D86">
         <v>88</v>
       </c>
-      <c r="E86" s="2">
+      <c r="E86">
         <v>92</v>
       </c>
       <c r="F86">
@@ -3437,10 +3435,10 @@
       <c r="C87" t="s">
         <v>245</v>
       </c>
-      <c r="D87" s="2">
+      <c r="D87">
         <v>81</v>
       </c>
-      <c r="E87" s="2">
+      <c r="E87">
         <v>99</v>
       </c>
       <c r="F87">
@@ -3460,10 +3458,10 @@
       <c r="C88" t="s">
         <v>248</v>
       </c>
-      <c r="D88" s="2">
+      <c r="D88">
         <v>48</v>
       </c>
-      <c r="E88" s="2">
+      <c r="E88">
         <v>65</v>
       </c>
       <c r="F88">
@@ -3483,10 +3481,10 @@
       <c r="C89" t="s">
         <v>251</v>
       </c>
-      <c r="D89" s="2">
+      <c r="D89">
         <v>79</v>
       </c>
-      <c r="E89" s="2">
+      <c r="E89">
         <v>56</v>
       </c>
       <c r="F89">
@@ -3506,10 +3504,10 @@
       <c r="C90" t="s">
         <v>253</v>
       </c>
-      <c r="D90" s="2">
+      <c r="D90">
         <v>20</v>
       </c>
-      <c r="E90" s="2">
+      <c r="E90">
         <v>29</v>
       </c>
       <c r="F90">
@@ -3529,10 +3527,10 @@
       <c r="C91" t="s">
         <v>256</v>
       </c>
-      <c r="D91" s="2">
+      <c r="D91">
         <v>62</v>
       </c>
-      <c r="E91" s="2">
+      <c r="E91">
         <v>75</v>
       </c>
       <c r="F91">
@@ -3552,10 +3550,10 @@
       <c r="C92" t="s">
         <v>259</v>
       </c>
-      <c r="D92" s="2">
+      <c r="D92">
         <v>57</v>
       </c>
-      <c r="E92" s="2">
+      <c r="E92">
         <v>40</v>
       </c>
       <c r="F92">
@@ -3575,10 +3573,10 @@
       <c r="C93" t="s">
         <v>262</v>
       </c>
-      <c r="D93" s="2">
+      <c r="D93">
         <v>100</v>
       </c>
-      <c r="E93" s="2">
+      <c r="E93">
         <v>95</v>
       </c>
       <c r="F93">
@@ -3598,10 +3596,10 @@
       <c r="C94" t="s">
         <v>265</v>
       </c>
-      <c r="D94" s="2">
+      <c r="D94">
         <v>69</v>
       </c>
-      <c r="E94" s="2">
+      <c r="E94">
         <v>83</v>
       </c>
       <c r="F94">
@@ -3621,10 +3619,10 @@
       <c r="C95" t="s">
         <v>268</v>
       </c>
-      <c r="D95" s="2">
+      <c r="D95">
         <v>71</v>
       </c>
-      <c r="E95" s="2">
+      <c r="E95">
         <v>67</v>
       </c>
       <c r="F95">
@@ -3644,10 +3642,10 @@
       <c r="C96" t="s">
         <v>270</v>
       </c>
-      <c r="D96" s="2">
+      <c r="D96">
         <v>48</v>
       </c>
-      <c r="E96" s="2">
+      <c r="E96">
         <v>61</v>
       </c>
       <c r="F96">
@@ -3667,10 +3665,10 @@
       <c r="C97" t="s">
         <v>273</v>
       </c>
-      <c r="D97" s="2">
+      <c r="D97">
         <v>73</v>
       </c>
-      <c r="E97" s="2">
+      <c r="E97">
         <v>97</v>
       </c>
       <c r="F97">
@@ -3690,10 +3688,10 @@
       <c r="C98" t="s">
         <v>276</v>
       </c>
-      <c r="D98" s="2">
+      <c r="D98">
         <v>94</v>
       </c>
-      <c r="E98" s="2">
+      <c r="E98">
         <v>67</v>
       </c>
       <c r="F98">
@@ -3713,10 +3711,10 @@
       <c r="C99" t="s">
         <v>279</v>
       </c>
-      <c r="D99" s="2">
+      <c r="D99">
         <v>89</v>
       </c>
-      <c r="E99" s="2">
+      <c r="E99">
         <v>78</v>
       </c>
       <c r="F99">
@@ -3736,10 +3734,10 @@
       <c r="C100" t="s">
         <v>282</v>
       </c>
-      <c r="D100" s="2">
+      <c r="D100">
         <v>93</v>
       </c>
-      <c r="E100" s="2">
+      <c r="E100">
         <v>94</v>
       </c>
       <c r="F100">
@@ -3759,10 +3757,10 @@
       <c r="C101" t="s">
         <v>285</v>
       </c>
-      <c r="D101" s="2">
+      <c r="D101">
         <v>86</v>
       </c>
-      <c r="E101" s="2">
+      <c r="E101">
         <v>95</v>
       </c>
       <c r="F101">
@@ -3782,10 +3780,10 @@
       <c r="C102" t="s">
         <v>288</v>
       </c>
-      <c r="D102" s="2">
+      <c r="D102">
         <v>63</v>
       </c>
-      <c r="E102" s="2">
+      <c r="E102">
         <v>67</v>
       </c>
       <c r="F102">
@@ -3805,10 +3803,10 @@
       <c r="C103" t="s">
         <v>291</v>
       </c>
-      <c r="D103" s="2">
+      <c r="D103">
         <v>70</v>
       </c>
-      <c r="E103" s="2">
+      <c r="E103">
         <v>38</v>
       </c>
       <c r="F103">
@@ -3828,10 +3826,10 @@
       <c r="C104" t="s">
         <v>294</v>
       </c>
-      <c r="D104" s="2">
+      <c r="D104">
         <v>67</v>
       </c>
-      <c r="E104" s="2">
+      <c r="E104">
         <v>45</v>
       </c>
       <c r="F104">
@@ -3851,10 +3849,10 @@
       <c r="C105" t="s">
         <v>297</v>
       </c>
-      <c r="D105" s="2">
+      <c r="D105">
         <v>86</v>
       </c>
-      <c r="E105" s="2">
+      <c r="E105">
         <v>73</v>
       </c>
       <c r="F105">
@@ -3874,10 +3872,10 @@
       <c r="C106" t="s">
         <v>300</v>
       </c>
-      <c r="D106" s="2">
+      <c r="D106">
         <v>76</v>
       </c>
-      <c r="E106" s="2">
+      <c r="E106">
         <v>88</v>
       </c>
       <c r="F106">
@@ -3897,10 +3895,10 @@
       <c r="C107" t="s">
         <v>302</v>
       </c>
-      <c r="D107" s="2">
+      <c r="D107">
         <v>74</v>
       </c>
-      <c r="E107" s="2">
+      <c r="E107">
         <v>38</v>
       </c>
       <c r="F107">
@@ -3920,10 +3918,10 @@
       <c r="C108" t="s">
         <v>304</v>
       </c>
-      <c r="D108" s="2">
+      <c r="D108">
         <v>86</v>
       </c>
-      <c r="E108" s="2">
+      <c r="E108">
         <v>94</v>
       </c>
       <c r="F108">
@@ -3943,10 +3941,10 @@
       <c r="C109" t="s">
         <v>307</v>
       </c>
-      <c r="D109" s="2">
+      <c r="D109">
         <v>83</v>
       </c>
-      <c r="E109" s="2">
+      <c r="E109">
         <v>63</v>
       </c>
       <c r="F109">
@@ -3966,10 +3964,10 @@
       <c r="C110" t="s">
         <v>309</v>
       </c>
-      <c r="D110" s="2">
+      <c r="D110">
         <v>93</v>
       </c>
-      <c r="E110" s="2">
+      <c r="E110">
         <v>91</v>
       </c>
       <c r="F110">
@@ -3989,10 +3987,10 @@
       <c r="C111" t="s">
         <v>311</v>
       </c>
-      <c r="D111" s="2">
+      <c r="D111">
         <v>88</v>
       </c>
-      <c r="E111" s="2">
+      <c r="E111">
         <v>94</v>
       </c>
       <c r="F111">
@@ -4012,10 +4010,10 @@
       <c r="C112" t="s">
         <v>313</v>
       </c>
-      <c r="D112" s="2">
+      <c r="D112">
         <v>47</v>
       </c>
-      <c r="E112" s="2">
+      <c r="E112">
         <v>57</v>
       </c>
       <c r="F112">
@@ -4035,10 +4033,10 @@
       <c r="C113" t="s">
         <v>316</v>
       </c>
-      <c r="D113" s="2">
+      <c r="D113">
         <v>60</v>
       </c>
-      <c r="E113" s="2">
+      <c r="E113">
         <v>90</v>
       </c>
       <c r="F113">
@@ -4058,10 +4056,10 @@
       <c r="C114" t="s">
         <v>319</v>
       </c>
-      <c r="D114" s="2">
+      <c r="D114">
         <v>98</v>
       </c>
-      <c r="E114" s="2">
+      <c r="E114">
         <v>93</v>
       </c>
       <c r="F114">
@@ -4081,10 +4079,10 @@
       <c r="C115" t="s">
         <v>322</v>
       </c>
-      <c r="D115" s="2">
+      <c r="D115">
         <v>82</v>
       </c>
-      <c r="E115" s="2">
+      <c r="E115">
         <v>86</v>
       </c>
       <c r="F115">
@@ -4104,10 +4102,10 @@
       <c r="C116" t="s">
         <v>325</v>
       </c>
-      <c r="D116" s="2">
+      <c r="D116">
         <v>62</v>
       </c>
-      <c r="E116" s="2">
+      <c r="E116">
         <v>63</v>
       </c>
       <c r="F116">
@@ -4127,10 +4125,10 @@
       <c r="C117" t="s">
         <v>327</v>
       </c>
-      <c r="D117" s="2">
+      <c r="D117">
         <v>94</v>
       </c>
-      <c r="E117" s="2">
+      <c r="E117">
         <v>82</v>
       </c>
       <c r="F117">
@@ -4150,10 +4148,10 @@
       <c r="C118" t="s">
         <v>330</v>
       </c>
-      <c r="D118" s="2">
+      <c r="D118">
         <v>69</v>
       </c>
-      <c r="E118" s="2">
+      <c r="E118">
         <v>54</v>
       </c>
       <c r="F118">
@@ -4164,50 +4162,50 @@
       </c>
     </row>
     <row r="119" spans="1:8" ht="15">
-      <c r="A119" s="3" t="s">
+      <c r="A119" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B119" s="3" t="s">
+      <c r="B119" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C119" s="3" t="s">
+      <c r="C119" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D119" s="4">
+      <c r="D119" s="3">
         <v>33</v>
       </c>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3">
-        <v>0</v>
-      </c>
-      <c r="G119" s="3">
-        <v>1</v>
-      </c>
-      <c r="H119" s="6" t="s">
+      <c r="E119" s="2"/>
+      <c r="F119" s="2">
+        <v>0</v>
+      </c>
+      <c r="G119" s="2">
+        <v>1</v>
+      </c>
+      <c r="H119" s="5" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="120" spans="1:8" ht="15">
-      <c r="A120" s="3" t="s">
+      <c r="A120" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="B120" s="3" t="s">
+      <c r="B120" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="C120" s="3" t="s">
+      <c r="C120" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="D120" s="3"/>
-      <c r="E120" s="4">
+      <c r="D120" s="2"/>
+      <c r="E120" s="3">
         <v>87</v>
       </c>
-      <c r="F120" s="3">
-        <v>1</v>
-      </c>
-      <c r="G120" s="3">
-        <v>1</v>
-      </c>
-      <c r="H120" s="6" t="s">
+      <c r="F120" s="2">
+        <v>1</v>
+      </c>
+      <c r="G120" s="2">
+        <v>1</v>
+      </c>
+      <c r="H120" s="5" t="s">
         <v>332</v>
       </c>
     </row>

</xml_diff>

<commit_message>
:art: Fixed an error get_entropy() method
Should be "+", typed "-"
</commit_message>
<xml_diff>
--- a/rotten_tomatoes/movie_list/movie_data.xlsx
+++ b/rotten_tomatoes/movie_list/movie_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangyanzhen/Developer/GitHub/CISC3014-IR-and-WebSearch-Project/rotten_tomatoes/movie_list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C530F9E-569B-584E-AF22-F3FE4067D7BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFCF701-AEC9-DB41-AF3C-4289CDB9FB52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="38360" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="367" uniqueCount="333">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="327">
   <si>
     <t>title</t>
   </si>
@@ -271,15 +271,6 @@
     <t>/m/1112549-crossroads</t>
   </si>
   <si>
-    <t>SexandtheFuture</t>
-  </si>
-  <si>
-    <t>Mar17,2020</t>
-  </si>
-  <si>
-    <t>/m/sex_and_the_future</t>
-  </si>
-  <si>
     <t>Attachment</t>
   </si>
   <si>
@@ -487,15 +478,9 @@
     <t>/m/sick_2022</t>
   </si>
   <si>
-    <t>Nyad</t>
-  </si>
-  <si>
     <t>Nov3,2023</t>
   </si>
   <si>
-    <t>/m/nyad</t>
-  </si>
-  <si>
     <t>Pearl</t>
   </si>
   <si>
@@ -1016,18 +1001,14 @@
   </si>
   <si>
     <t>bad data</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>YES</t>
-    <phoneticPr fontId="3" type="noConversion"/>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1043,14 +1024,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <family val="2"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="9"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -1058,17 +1031,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -1106,28 +1074,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="差" xfId="1" builtinId="27"/>
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1428,10 +1387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H120"/>
+  <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P36" sqref="P36"/>
+    <sheetView tabSelected="1" topLeftCell="A95" workbookViewId="0">
+      <selection activeCell="M117" sqref="M117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
@@ -1466,8 +1425,8 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
-        <v>331</v>
+      <c r="H1" s="2" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -2116,13 +2075,13 @@
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="B30" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C30" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D30">
         <v>59</v>
@@ -2139,13 +2098,13 @@
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="D31">
         <v>73</v>
@@ -2162,13 +2121,13 @@
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B32" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C32" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D32">
         <v>78</v>
@@ -2185,13 +2144,13 @@
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B33" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C33" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D33">
         <v>75</v>
@@ -2208,13 +2167,13 @@
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B34" t="s">
         <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D34">
         <v>99</v>
@@ -2231,13 +2190,13 @@
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B35" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C35" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D35">
         <v>66</v>
@@ -2254,13 +2213,13 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B36" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C36" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="D36">
         <v>86</v>
@@ -2277,13 +2236,13 @@
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B37" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C37" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D37">
         <v>92</v>
@@ -2300,13 +2259,13 @@
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C38" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D38">
         <v>92</v>
@@ -2323,13 +2282,13 @@
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="B39" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D39">
         <v>76</v>
@@ -2346,13 +2305,13 @@
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B40" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C40" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D40">
         <v>70</v>
@@ -2369,13 +2328,13 @@
     </row>
     <row r="41" spans="1:7">
       <c r="A41" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B41" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="C41" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D41">
         <v>68</v>
@@ -2392,13 +2351,13 @@
     </row>
     <row r="42" spans="1:7">
       <c r="A42" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B42" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D42">
         <v>94</v>
@@ -2415,13 +2374,13 @@
     </row>
     <row r="43" spans="1:7">
       <c r="A43" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B43" t="s">
         <v>22</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D43">
         <v>88</v>
@@ -2438,13 +2397,13 @@
     </row>
     <row r="44" spans="1:7">
       <c r="A44" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B44" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C44" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D44">
         <v>61</v>
@@ -2461,13 +2420,13 @@
     </row>
     <row r="45" spans="1:7">
       <c r="A45" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B45" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C45" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D45">
         <v>89</v>
@@ -2484,13 +2443,13 @@
     </row>
     <row r="46" spans="1:7">
       <c r="A46" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B46" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C46" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="D46">
         <v>52</v>
@@ -2507,13 +2466,13 @@
     </row>
     <row r="47" spans="1:7">
       <c r="A47" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B47" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C47" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D47">
         <v>98</v>
@@ -2530,13 +2489,13 @@
     </row>
     <row r="48" spans="1:7">
       <c r="A48" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B48" t="s">
         <v>25</v>
       </c>
       <c r="C48" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D48">
         <v>53</v>
@@ -2553,13 +2512,13 @@
     </row>
     <row r="49" spans="1:7">
       <c r="A49" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B49" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C49" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D49">
         <v>14</v>
@@ -2576,13 +2535,13 @@
     </row>
     <row r="50" spans="1:7">
       <c r="A50" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B50" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C50" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D50">
         <v>98</v>
@@ -2599,13 +2558,13 @@
     </row>
     <row r="51" spans="1:7">
       <c r="A51" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B51" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C51" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D51">
         <v>71</v>
@@ -2622,13 +2581,13 @@
     </row>
     <row r="52" spans="1:7">
       <c r="A52" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B52" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C52" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D52">
         <v>81</v>
@@ -2645,13 +2604,13 @@
     </row>
     <row r="53" spans="1:7">
       <c r="A53" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="B53" t="s">
+        <v>145</v>
+      </c>
+      <c r="C53" t="s">
         <v>148</v>
-      </c>
-      <c r="C53" t="s">
-        <v>151</v>
       </c>
       <c r="D53">
         <v>79</v>
@@ -2668,13 +2627,13 @@
     </row>
     <row r="54" spans="1:7">
       <c r="A54" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B54" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C54" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="D54">
         <v>74</v>
@@ -2691,13 +2650,13 @@
     </row>
     <row r="55" spans="1:7">
       <c r="A55" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B55" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C55" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="D55">
         <v>82</v>
@@ -2714,13 +2673,13 @@
     </row>
     <row r="56" spans="1:7">
       <c r="A56" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B56" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C56" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D56">
         <v>89</v>
@@ -2737,13 +2696,13 @@
     </row>
     <row r="57" spans="1:7">
       <c r="A57" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B57" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C57" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="D57">
         <v>35</v>
@@ -2760,13 +2719,13 @@
     </row>
     <row r="58" spans="1:7">
       <c r="A58" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B58" t="s">
         <v>37</v>
       </c>
       <c r="C58" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D58">
         <v>50</v>
@@ -2783,13 +2742,13 @@
     </row>
     <row r="59" spans="1:7">
       <c r="A59" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B59" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C59" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D59">
         <v>50</v>
@@ -2806,13 +2765,13 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B60" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C60" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="D60">
         <v>72</v>
@@ -2829,13 +2788,13 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="B61" t="s">
         <v>25</v>
       </c>
       <c r="C61" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="D61">
         <v>71</v>
@@ -2852,13 +2811,13 @@
     </row>
     <row r="62" spans="1:7">
       <c r="A62" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="B62" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="C62" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="D62">
         <v>73</v>
@@ -2875,13 +2834,13 @@
     </row>
     <row r="63" spans="1:7">
       <c r="A63" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B63" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C63" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="D63">
         <v>84</v>
@@ -2898,13 +2857,13 @@
     </row>
     <row r="64" spans="1:7">
       <c r="A64" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="B64" t="s">
         <v>13</v>
       </c>
       <c r="C64" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="D64">
         <v>93</v>
@@ -2921,13 +2880,13 @@
     </row>
     <row r="65" spans="1:7">
       <c r="A65" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B65" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C65" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D65">
         <v>94</v>
@@ -2944,13 +2903,13 @@
     </row>
     <row r="66" spans="1:7">
       <c r="A66" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="B66" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="C66" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="D66">
         <v>75</v>
@@ -2967,13 +2926,13 @@
     </row>
     <row r="67" spans="1:7">
       <c r="A67" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="B67" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C67" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D67">
         <v>75</v>
@@ -2990,13 +2949,13 @@
     </row>
     <row r="68" spans="1:7">
       <c r="A68" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="B68" t="s">
         <v>42</v>
       </c>
       <c r="C68" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="D68">
         <v>54</v>
@@ -3013,13 +2972,13 @@
     </row>
     <row r="69" spans="1:7">
       <c r="A69" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B69" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="C69" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="D69">
         <v>60</v>
@@ -3036,13 +2995,13 @@
     </row>
     <row r="70" spans="1:7">
       <c r="A70" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="B70" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="C70" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="D70">
         <v>89</v>
@@ -3059,13 +3018,13 @@
     </row>
     <row r="71" spans="1:7">
       <c r="A71" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="B71" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="C71" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="D71">
         <v>65</v>
@@ -3082,13 +3041,13 @@
     </row>
     <row r="72" spans="1:7">
       <c r="A72" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="B72" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C72" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="D72">
         <v>69</v>
@@ -3105,13 +3064,13 @@
     </row>
     <row r="73" spans="1:7">
       <c r="A73" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="B73" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="C73" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="D73">
         <v>91</v>
@@ -3128,13 +3087,13 @@
     </row>
     <row r="74" spans="1:7">
       <c r="A74" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="B74" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="C74" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="D74">
         <v>73</v>
@@ -3151,13 +3110,13 @@
     </row>
     <row r="75" spans="1:7">
       <c r="A75" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="B75" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="C75" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="D75">
         <v>88</v>
@@ -3174,13 +3133,13 @@
     </row>
     <row r="76" spans="1:7">
       <c r="A76" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="B76" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C76" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="D76">
         <v>89</v>
@@ -3197,13 +3156,13 @@
     </row>
     <row r="77" spans="1:7">
       <c r="A77" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="B77" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C77" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D77">
         <v>62</v>
@@ -3220,13 +3179,13 @@
     </row>
     <row r="78" spans="1:7">
       <c r="A78" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="B78" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C78" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="D78">
         <v>77</v>
@@ -3243,13 +3202,13 @@
     </row>
     <row r="79" spans="1:7">
       <c r="A79" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B79" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C79" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="D79">
         <v>85</v>
@@ -3266,13 +3225,13 @@
     </row>
     <row r="80" spans="1:7">
       <c r="A80" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="B80" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="C80" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D80">
         <v>71</v>
@@ -3289,13 +3248,13 @@
     </row>
     <row r="81" spans="1:7">
       <c r="A81" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B81" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="C81" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D81">
         <v>95</v>
@@ -3312,13 +3271,13 @@
     </row>
     <row r="82" spans="1:7">
       <c r="A82" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="B82" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="C82" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D82">
         <v>93</v>
@@ -3335,13 +3294,13 @@
     </row>
     <row r="83" spans="1:7">
       <c r="A83" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="B83" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C83" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D83">
         <v>70</v>
@@ -3358,13 +3317,13 @@
     </row>
     <row r="84" spans="1:7">
       <c r="A84" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B84" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="C84" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D84">
         <v>90</v>
@@ -3381,13 +3340,13 @@
     </row>
     <row r="85" spans="1:7">
       <c r="A85" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="B85" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="C85" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D85">
         <v>72</v>
@@ -3404,13 +3363,13 @@
     </row>
     <row r="86" spans="1:7">
       <c r="A86" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="B86" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="C86" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D86">
         <v>88</v>
@@ -3427,13 +3386,13 @@
     </row>
     <row r="87" spans="1:7">
       <c r="A87" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B87" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="C87" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D87">
         <v>81</v>
@@ -3450,13 +3409,13 @@
     </row>
     <row r="88" spans="1:7">
       <c r="A88" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B88" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="C88" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D88">
         <v>48</v>
@@ -3473,13 +3432,13 @@
     </row>
     <row r="89" spans="1:7">
       <c r="A89" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="B89" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="C89" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D89">
         <v>79</v>
@@ -3496,13 +3455,13 @@
     </row>
     <row r="90" spans="1:7">
       <c r="A90" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B90" t="s">
         <v>8</v>
       </c>
       <c r="C90" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D90">
         <v>20</v>
@@ -3519,13 +3478,13 @@
     </row>
     <row r="91" spans="1:7">
       <c r="A91" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B91" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="C91" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D91">
         <v>62</v>
@@ -3542,13 +3501,13 @@
     </row>
     <row r="92" spans="1:7">
       <c r="A92" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B92" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="C92" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D92">
         <v>57</v>
@@ -3565,13 +3524,13 @@
     </row>
     <row r="93" spans="1:7">
       <c r="A93" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B93" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="C93" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D93">
         <v>100</v>
@@ -3588,13 +3547,13 @@
     </row>
     <row r="94" spans="1:7">
       <c r="A94" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="B94" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C94" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D94">
         <v>69</v>
@@ -3611,13 +3570,13 @@
     </row>
     <row r="95" spans="1:7">
       <c r="A95" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="B95" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="C95" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D95">
         <v>71</v>
@@ -3634,13 +3593,13 @@
     </row>
     <row r="96" spans="1:7">
       <c r="A96" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="B96" t="s">
         <v>59</v>
       </c>
       <c r="C96" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D96">
         <v>48</v>
@@ -3657,13 +3616,13 @@
     </row>
     <row r="97" spans="1:7">
       <c r="A97" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="B97" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C97" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D97">
         <v>73</v>
@@ -3680,13 +3639,13 @@
     </row>
     <row r="98" spans="1:7">
       <c r="A98" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="B98" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C98" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D98">
         <v>94</v>
@@ -3703,13 +3662,13 @@
     </row>
     <row r="99" spans="1:7">
       <c r="A99" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="B99" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="C99" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D99">
         <v>89</v>
@@ -3726,13 +3685,13 @@
     </row>
     <row r="100" spans="1:7">
       <c r="A100" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B100" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="C100" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D100">
         <v>93</v>
@@ -3749,13 +3708,13 @@
     </row>
     <row r="101" spans="1:7">
       <c r="A101" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="B101" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="C101" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D101">
         <v>86</v>
@@ -3772,13 +3731,13 @@
     </row>
     <row r="102" spans="1:7">
       <c r="A102" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="B102" t="s">
-        <v>287</v>
+        <v>282</v>
       </c>
       <c r="C102" t="s">
-        <v>288</v>
+        <v>283</v>
       </c>
       <c r="D102">
         <v>63</v>
@@ -3795,13 +3754,13 @@
     </row>
     <row r="103" spans="1:7">
       <c r="A103" t="s">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B103" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="C103" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="D103">
         <v>70</v>
@@ -3818,13 +3777,13 @@
     </row>
     <row r="104" spans="1:7">
       <c r="A104" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B104" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C104" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D104">
         <v>67</v>
@@ -3841,13 +3800,13 @@
     </row>
     <row r="105" spans="1:7">
       <c r="A105" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B105" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C105" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
       <c r="D105">
         <v>86</v>
@@ -3864,13 +3823,13 @@
     </row>
     <row r="106" spans="1:7">
       <c r="A106" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="B106" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="C106" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D106">
         <v>76</v>
@@ -3887,13 +3846,13 @@
     </row>
     <row r="107" spans="1:7">
       <c r="A107" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="B107" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C107" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="D107">
         <v>74</v>
@@ -3910,13 +3869,13 @@
     </row>
     <row r="108" spans="1:7">
       <c r="A108" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="B108" t="s">
         <v>37</v>
       </c>
       <c r="C108" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D108">
         <v>86</v>
@@ -3933,13 +3892,13 @@
     </row>
     <row r="109" spans="1:7">
       <c r="A109" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="B109" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C109" t="s">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="D109">
         <v>83</v>
@@ -3956,13 +3915,13 @@
     </row>
     <row r="110" spans="1:7">
       <c r="A110" t="s">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="B110" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C110" t="s">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="D110">
         <v>93</v>
@@ -3979,13 +3938,13 @@
     </row>
     <row r="111" spans="1:7">
       <c r="A111" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="B111" t="s">
         <v>34</v>
       </c>
       <c r="C111" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D111">
         <v>88</v>
@@ -4002,13 +3961,13 @@
     </row>
     <row r="112" spans="1:7">
       <c r="A112" t="s">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="B112" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="C112" t="s">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="D112">
         <v>47</v>
@@ -4023,15 +3982,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:8">
+    <row r="113" spans="1:7">
       <c r="A113" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="B113" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C113" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="D113">
         <v>60</v>
@@ -4046,15 +4005,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:8">
+    <row r="114" spans="1:7">
       <c r="A114" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="B114" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C114" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="D114">
         <v>98</v>
@@ -4069,15 +4028,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:8">
+    <row r="115" spans="1:7">
       <c r="A115" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B115" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C115" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
       <c r="D115">
         <v>82</v>
@@ -4092,15 +4051,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:8">
+    <row r="116" spans="1:7">
       <c r="A116" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B116" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C116" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D116">
         <v>62</v>
@@ -4115,15 +4074,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:8">
+    <row r="117" spans="1:7">
       <c r="A117" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="B117" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="C117" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
       <c r="D117">
         <v>94</v>
@@ -4138,15 +4097,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:8">
+    <row r="118" spans="1:7">
       <c r="A118" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
       <c r="B118" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C118" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="D118">
         <v>69</v>
@@ -4161,56 +4120,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:8" ht="15">
-      <c r="A119" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="B119" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C119" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D119" s="3">
-        <v>33</v>
-      </c>
-      <c r="E119" s="2"/>
-      <c r="F119" s="2">
-        <v>0</v>
-      </c>
-      <c r="G119" s="2">
-        <v>1</v>
-      </c>
-      <c r="H119" s="5" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" ht="15">
-      <c r="A120" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="B120" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="C120" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="D120" s="2"/>
-      <c r="E120" s="3">
-        <v>87</v>
-      </c>
-      <c r="F120" s="2">
-        <v>1</v>
-      </c>
-      <c r="G120" s="2">
-        <v>1</v>
-      </c>
-      <c r="H120" s="5" t="s">
-        <v>332</v>
-      </c>
-    </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
:new: Added tf-idf analysis
</commit_message>
<xml_diff>
--- a/rotten_tomatoes/movie_list/movie_data.xlsx
+++ b/rotten_tomatoes/movie_list/movie_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/huangyanzhen/Developer/GitHub/CISC3014-IR-and-WebSearch-Project/rotten_tomatoes/movie_list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D8D6184-FA7D-8543-BDC9-A7420E9245A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03276389-11D2-754B-A524-BE7F6689280C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="38360" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1390,14 +1390,14 @@
   <dimension ref="A1:H118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="43.6640625" customWidth="1"/>
     <col min="2" max="2" width="17.6640625" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="27.83203125" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="27.83203125" customWidth="1"/>
     <col min="4" max="4" width="21.33203125" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="20.1640625" customWidth="1"/>

</xml_diff>